<commit_message>
Added Summation for the 2 rows
</commit_message>
<xml_diff>
--- a/diabetes_data.xlsx
+++ b/diabetes_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1596" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1598" uniqueCount="20">
   <si>
     <t>Index</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>Weight</t>
+  </si>
+  <si>
+    <t>BC</t>
   </si>
 </sst>
 </file>
@@ -63514,13 +63517,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N21"/>
+  <dimension ref="A1:AD22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:30">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -63563,8 +63566,56 @@
       <c r="N1" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:14">
+      <c r="O1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>1</v>
+      </c>
+      <c r="R1" s="1">
+        <v>2</v>
+      </c>
+      <c r="S1" s="1">
+        <v>3</v>
+      </c>
+      <c r="T1" s="1">
+        <v>4</v>
+      </c>
+      <c r="U1" s="1">
+        <v>5</v>
+      </c>
+      <c r="V1" s="1">
+        <v>6</v>
+      </c>
+      <c r="W1" s="1">
+        <v>7</v>
+      </c>
+      <c r="X1" s="1">
+        <v>8</v>
+      </c>
+      <c r="Y1" s="1">
+        <v>9</v>
+      </c>
+      <c r="Z1" s="1">
+        <v>10</v>
+      </c>
+      <c r="AA1" s="1">
+        <v>11</v>
+      </c>
+      <c r="AB1" s="1">
+        <v>12</v>
+      </c>
+      <c r="AC1" s="1">
+        <v>13</v>
+      </c>
+      <c r="AD1" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30">
       <c r="A2">
         <v>0</v>
       </c>
@@ -63607,8 +63658,11 @@
       <c r="N2">
         <v>228.2228732935722</v>
       </c>
-    </row>
-    <row r="3" spans="1:14">
+      <c r="O2">
+        <v>7.643466364614945</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30">
       <c r="A3">
         <v>1</v>
       </c>
@@ -63651,8 +63705,11 @@
       <c r="N3">
         <v>155.5228900833753</v>
       </c>
-    </row>
-    <row r="4" spans="1:14">
+      <c r="O3">
+        <v>5.811543587034343</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30">
       <c r="A4">
         <v>0</v>
       </c>
@@ -63695,8 +63752,11 @@
       <c r="N4">
         <v>228.2228732935722</v>
       </c>
-    </row>
-    <row r="5" spans="1:14">
+      <c r="O4">
+        <v>7.643466364614945</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30">
       <c r="A5">
         <v>2</v>
       </c>
@@ -63739,8 +63799,11 @@
       <c r="N5">
         <v>230.6932436063973</v>
       </c>
-    </row>
-    <row r="6" spans="1:14">
+      <c r="O5">
+        <v>6.484216255801467</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30">
       <c r="A6">
         <v>0</v>
       </c>
@@ -63783,8 +63846,11 @@
       <c r="N6">
         <v>228.2228732935722</v>
       </c>
-    </row>
-    <row r="7" spans="1:14">
+      <c r="O6">
+        <v>7.643466364614945</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30">
       <c r="A7">
         <v>3</v>
       </c>
@@ -63827,8 +63893,11 @@
       <c r="N7">
         <v>140.7546366721272</v>
       </c>
-    </row>
-    <row r="8" spans="1:14">
+      <c r="O7">
+        <v>4.877338801231672</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30">
       <c r="A8">
         <v>0</v>
       </c>
@@ -63871,8 +63940,11 @@
       <c r="N8">
         <v>228.2228732935722</v>
       </c>
-    </row>
-    <row r="9" spans="1:14">
+      <c r="O8">
+        <v>7.643466364614945</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30">
       <c r="A9">
         <v>4</v>
       </c>
@@ -63915,8 +63987,11 @@
       <c r="N9">
         <v>172.4093614298593</v>
       </c>
-    </row>
-    <row r="10" spans="1:14">
+      <c r="O9">
+        <v>6.012852133638411</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30">
       <c r="A10">
         <v>1</v>
       </c>
@@ -63959,8 +64034,11 @@
       <c r="N10">
         <v>155.5228900833753</v>
       </c>
-    </row>
-    <row r="11" spans="1:14">
+      <c r="O10">
+        <v>5.811543587034343</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30">
       <c r="A11">
         <v>2</v>
       </c>
@@ -64003,8 +64081,11 @@
       <c r="N11">
         <v>230.6932436063973</v>
       </c>
-    </row>
-    <row r="12" spans="1:14">
+      <c r="O11">
+        <v>6.484216255801467</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30">
       <c r="A12">
         <v>1</v>
       </c>
@@ -64047,8 +64128,11 @@
       <c r="N12">
         <v>155.5228900833753</v>
       </c>
-    </row>
-    <row r="13" spans="1:14">
+      <c r="O12">
+        <v>5.811543587034343</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30">
       <c r="A13">
         <v>3</v>
       </c>
@@ -64091,8 +64175,11 @@
       <c r="N13">
         <v>140.7546366721272</v>
       </c>
-    </row>
-    <row r="14" spans="1:14">
+      <c r="O13">
+        <v>4.877338801231672</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30">
       <c r="A14">
         <v>1</v>
       </c>
@@ -64135,8 +64222,11 @@
       <c r="N14">
         <v>155.5228900833753</v>
       </c>
-    </row>
-    <row r="15" spans="1:14">
+      <c r="O14">
+        <v>5.811543587034343</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30">
       <c r="A15">
         <v>4</v>
       </c>
@@ -64179,8 +64269,11 @@
       <c r="N15">
         <v>172.4093614298593</v>
       </c>
-    </row>
-    <row r="16" spans="1:14">
+      <c r="O15">
+        <v>6.012852133638411</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30">
       <c r="A16">
         <v>2</v>
       </c>
@@ -64223,8 +64316,11 @@
       <c r="N16">
         <v>230.6932436063973</v>
       </c>
-    </row>
-    <row r="17" spans="1:14">
+      <c r="O16">
+        <v>6.484216255801467</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30">
       <c r="A17">
         <v>3</v>
       </c>
@@ -64267,8 +64363,11 @@
       <c r="N17">
         <v>140.7546366721272</v>
       </c>
-    </row>
-    <row r="18" spans="1:14">
+      <c r="O17">
+        <v>4.877338801231672</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30">
       <c r="A18">
         <v>2</v>
       </c>
@@ -64311,8 +64410,11 @@
       <c r="N18">
         <v>230.6932436063973</v>
       </c>
-    </row>
-    <row r="19" spans="1:14">
+      <c r="O18">
+        <v>6.484216255801467</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30">
       <c r="A19">
         <v>4</v>
       </c>
@@ -64355,8 +64457,11 @@
       <c r="N19">
         <v>172.4093614298593</v>
       </c>
-    </row>
-    <row r="20" spans="1:14">
+      <c r="O19">
+        <v>6.012852133638411</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30">
       <c r="A20">
         <v>3</v>
       </c>
@@ -64399,8 +64504,11 @@
       <c r="N20">
         <v>140.7546366721272</v>
       </c>
-    </row>
-    <row r="21" spans="1:14">
+      <c r="O20">
+        <v>4.877338801231672</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30">
       <c r="A21">
         <v>4</v>
       </c>
@@ -64442,6 +64550,56 @@
       </c>
       <c r="N21">
         <v>172.4093614298593</v>
+      </c>
+      <c r="O21">
+        <v>6.012852133638411</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30">
+      <c r="P22">
+        <v>7</v>
+      </c>
+      <c r="Q22">
+        <v>1</v>
+      </c>
+      <c r="R22">
+        <v>1.135678392</v>
+      </c>
+      <c r="S22">
+        <v>0.868852459</v>
+      </c>
+      <c r="T22">
+        <v>0.5858585860000001</v>
+      </c>
+      <c r="U22">
+        <v>0.309692671</v>
+      </c>
+      <c r="V22">
+        <v>1.061102831</v>
+      </c>
+      <c r="W22">
+        <v>0.981639624</v>
+      </c>
+      <c r="X22">
+        <v>54</v>
+      </c>
+      <c r="Y22">
+        <v>1</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA22">
+        <v>59.942824563</v>
+      </c>
+      <c r="AB22">
+        <v>0.8936291064282529</v>
+      </c>
+      <c r="AC22">
+        <v>313.1639981019865</v>
+      </c>
+      <c r="AD22">
+        <v>10.89019093487008</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added code for writing summation into thw sheet
</commit_message>
<xml_diff>
--- a/diabetes_data.xlsx
+++ b/diabetes_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1598" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1607" uniqueCount="23">
   <si>
     <t>Index</t>
   </si>
@@ -76,6 +76,15 @@
   </si>
   <si>
     <t>BC</t>
+  </si>
+  <si>
+    <t>BB</t>
+  </si>
+  <si>
+    <t>CB</t>
+  </si>
+  <si>
+    <t>CC</t>
   </si>
 </sst>
 </file>
@@ -63517,13 +63526,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AD22"/>
+  <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:30">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -63569,53 +63578,8 @@
       <c r="O1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="P1" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q1" s="1">
-        <v>1</v>
-      </c>
-      <c r="R1" s="1">
-        <v>2</v>
-      </c>
-      <c r="S1" s="1">
-        <v>3</v>
-      </c>
-      <c r="T1" s="1">
-        <v>4</v>
-      </c>
-      <c r="U1" s="1">
-        <v>5</v>
-      </c>
-      <c r="V1" s="1">
-        <v>6</v>
-      </c>
-      <c r="W1" s="1">
-        <v>7</v>
-      </c>
-      <c r="X1" s="1">
-        <v>8</v>
-      </c>
-      <c r="Y1" s="1">
-        <v>9</v>
-      </c>
-      <c r="Z1" s="1">
-        <v>10</v>
-      </c>
-      <c r="AA1" s="1">
-        <v>11</v>
-      </c>
-      <c r="AB1" s="1">
-        <v>12</v>
-      </c>
-      <c r="AC1" s="1">
-        <v>13</v>
-      </c>
-      <c r="AD1" s="1">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:30">
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2">
         <v>0</v>
       </c>
@@ -63662,7 +63626,7 @@
         <v>7.643466364614945</v>
       </c>
     </row>
-    <row r="3" spans="1:30">
+    <row r="3" spans="1:15">
       <c r="A3">
         <v>1</v>
       </c>
@@ -63709,80 +63673,80 @@
         <v>5.811543587034343</v>
       </c>
     </row>
-    <row r="4" spans="1:30">
+    <row r="4" spans="1:15">
       <c r="A4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B4">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>1.170854271</v>
+      </c>
+      <c r="D4">
+        <v>1.131147541</v>
+      </c>
+      <c r="E4">
+        <v>0.6464646469999999</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0.8971684049999999</v>
+      </c>
+      <c r="H4">
+        <v>0.350982067</v>
+      </c>
+      <c r="I4">
+        <v>81</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4">
+        <v>92.19661693099999</v>
+      </c>
+      <c r="M4">
+        <v>1.079129326212337</v>
+      </c>
+      <c r="N4">
+        <v>383.7457633769475</v>
+      </c>
+      <c r="O4">
+        <v>13.45500995164929</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
         <v>6</v>
       </c>
-      <c r="C4">
+      <c r="C5">
         <v>0.743718593</v>
       </c>
-      <c r="D4">
+      <c r="D5">
         <v>0.590163934</v>
       </c>
-      <c r="E4">
+      <c r="E5">
         <v>0.353535354</v>
       </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
         <v>0.500745156</v>
       </c>
-      <c r="H4">
+      <c r="H5">
         <v>0.23441503</v>
       </c>
-      <c r="I4">
+      <c r="I5">
         <v>50</v>
-      </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-      <c r="K4" t="s">
-        <v>11</v>
-      </c>
-      <c r="L4">
-        <v>58.422578067</v>
-      </c>
-      <c r="M4">
-        <v>0.6336737725498485</v>
-      </c>
-      <c r="N4">
-        <v>228.2228732935722</v>
-      </c>
-      <c r="O4">
-        <v>7.643466364614945</v>
-      </c>
-    </row>
-    <row r="5" spans="1:30">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5">
-        <v>8</v>
-      </c>
-      <c r="C5">
-        <v>0.91959799</v>
-      </c>
-      <c r="D5">
-        <v>0.524590164</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0.347242921</v>
-      </c>
-      <c r="H5">
-        <v>0.253629377</v>
-      </c>
-      <c r="I5">
-        <v>32</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -63791,45 +63755,45 @@
         <v>11</v>
       </c>
       <c r="L5">
-        <v>42.045060452</v>
+        <v>58.422578067</v>
       </c>
       <c r="M5">
-        <v>0.6386575851883864</v>
+        <v>0.6336737725498485</v>
       </c>
       <c r="N5">
-        <v>230.6932436063973</v>
+        <v>228.2228732935722</v>
       </c>
       <c r="O5">
-        <v>6.484216255801467</v>
-      </c>
-    </row>
-    <row r="6" spans="1:30">
+        <v>7.643466364614945</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B6">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C6">
-        <v>0.743718593</v>
+        <v>0.91959799</v>
       </c>
       <c r="D6">
-        <v>0.590163934</v>
+        <v>0.524590164</v>
       </c>
       <c r="E6">
-        <v>0.353535354</v>
+        <v>0</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>0.500745156</v>
+        <v>0.347242921</v>
       </c>
       <c r="H6">
-        <v>0.23441503</v>
+        <v>0.253629377</v>
       </c>
       <c r="I6">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="J6">
         <v>1</v>
@@ -63838,66 +63802,66 @@
         <v>11</v>
       </c>
       <c r="L6">
-        <v>58.422578067</v>
+        <v>42.045060452</v>
       </c>
       <c r="M6">
-        <v>0.6336737725498485</v>
+        <v>0.6386575851883864</v>
       </c>
       <c r="N6">
-        <v>228.2228732935722</v>
+        <v>230.6932436063973</v>
       </c>
       <c r="O6">
-        <v>7.643466364614945</v>
-      </c>
-    </row>
-    <row r="7" spans="1:30">
+        <v>6.484216255801467</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C7">
-        <v>0.447236181</v>
+        <v>1.663316583</v>
       </c>
       <c r="D7">
-        <v>0.540983607</v>
+        <v>1.114754098</v>
       </c>
       <c r="E7">
-        <v>0.232323232</v>
+        <v>0.353535354</v>
       </c>
       <c r="F7">
-        <v>0.111111111</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <v>0.418777943</v>
+        <v>0.847988077</v>
       </c>
       <c r="H7">
-        <v>0.038001708</v>
+        <v>0.488044407</v>
       </c>
       <c r="I7">
-        <v>21</v>
+        <v>82</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K7" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="L7">
-        <v>23.788433782</v>
+        <v>100.467638519</v>
       </c>
       <c r="M7">
-        <v>0.3968520662051606</v>
+        <v>1.272331357738235</v>
       </c>
       <c r="N7">
-        <v>140.7546366721272</v>
+        <v>458.9161168999695</v>
       </c>
       <c r="O7">
-        <v>4.877338801231672</v>
-      </c>
-    </row>
-    <row r="8" spans="1:30">
+        <v>14.12768262041641</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8">
         <v>0</v>
       </c>
@@ -63944,127 +63908,127 @@
         <v>7.643466364614945</v>
       </c>
     </row>
-    <row r="9" spans="1:30">
+    <row r="9" spans="1:15">
       <c r="A9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9">
-        <v>0.6884422109999999</v>
+        <v>0.447236181</v>
       </c>
       <c r="D9">
-        <v>0.327868852</v>
+        <v>0.540983607</v>
       </c>
       <c r="E9">
+        <v>0.232323232</v>
+      </c>
+      <c r="F9">
+        <v>0.111111111</v>
+      </c>
+      <c r="G9">
+        <v>0.418777943</v>
+      </c>
+      <c r="H9">
+        <v>0.038001708</v>
+      </c>
+      <c r="I9">
+        <v>21</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L9">
+        <v>23.788433782</v>
+      </c>
+      <c r="M9">
+        <v>0.3968520662051606</v>
+      </c>
+      <c r="N9">
+        <v>140.7546366721272</v>
+      </c>
+      <c r="O9">
+        <v>4.877338801231672</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <v>1.190954774</v>
+      </c>
+      <c r="D10">
+        <v>1.131147541</v>
+      </c>
+      <c r="E10">
+        <v>0.5858585860000001</v>
+      </c>
+      <c r="F10">
+        <v>0.111111111</v>
+      </c>
+      <c r="G10">
+        <v>0.9195230990000001</v>
+      </c>
+      <c r="H10">
+        <v>0.272416738</v>
+      </c>
+      <c r="I10">
+        <v>71</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10" t="s">
+        <v>20</v>
+      </c>
+      <c r="L10">
+        <v>82.211011849</v>
+      </c>
+      <c r="M10">
+        <v>1.030525838755009</v>
+      </c>
+      <c r="N10">
+        <v>368.9775099656994</v>
+      </c>
+      <c r="O10">
+        <v>12.52080516584662</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <v>0.743718593</v>
+      </c>
+      <c r="D11">
+        <v>0.590163934</v>
+      </c>
+      <c r="E11">
         <v>0.353535354</v>
       </c>
-      <c r="F9">
-        <v>0.19858156</v>
-      </c>
-      <c r="G9">
-        <v>0.642324888</v>
-      </c>
-      <c r="H9">
-        <v>0.943637916</v>
-      </c>
-      <c r="I9">
-        <v>33</v>
-      </c>
-      <c r="J9">
-        <v>1</v>
-      </c>
-      <c r="K9" t="s">
-        <v>12</v>
-      </c>
-      <c r="L9">
-        <v>36.154390781</v>
-      </c>
-      <c r="M9">
-        <v>0.4967770402230923</v>
-      </c>
-      <c r="N9">
-        <v>172.4093614298593</v>
-      </c>
-      <c r="O9">
-        <v>6.012852133638411</v>
-      </c>
-    </row>
-    <row r="10" spans="1:30">
-      <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>0.427135678</v>
-      </c>
-      <c r="D10">
-        <v>0.540983607</v>
-      </c>
-      <c r="E10">
-        <v>0.292929293</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0.396423249</v>
-      </c>
-      <c r="H10">
-        <v>0.116567037</v>
-      </c>
-      <c r="I10">
-        <v>31</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10" t="s">
-        <v>12</v>
-      </c>
-      <c r="L10">
-        <v>33.774038864</v>
-      </c>
-      <c r="M10">
-        <v>0.4454555536624887</v>
-      </c>
-      <c r="N10">
-        <v>155.5228900833753</v>
-      </c>
-      <c r="O10">
-        <v>5.811543587034343</v>
-      </c>
-    </row>
-    <row r="11" spans="1:30">
-      <c r="A11">
-        <v>2</v>
-      </c>
-      <c r="B11">
-        <v>8</v>
-      </c>
-      <c r="C11">
-        <v>0.91959799</v>
-      </c>
-      <c r="D11">
-        <v>0.524590164</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
       <c r="F11">
         <v>0</v>
       </c>
       <c r="G11">
-        <v>0.347242921</v>
+        <v>0.500745156</v>
       </c>
       <c r="H11">
-        <v>0.253629377</v>
+        <v>0.23441503</v>
       </c>
       <c r="I11">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="J11">
         <v>1</v>
@@ -64073,113 +64037,113 @@
         <v>11</v>
       </c>
       <c r="L11">
-        <v>42.045060452</v>
+        <v>58.422578067</v>
       </c>
       <c r="M11">
-        <v>0.6386575851883864</v>
+        <v>0.6336737725498485</v>
       </c>
       <c r="N11">
-        <v>230.6932436063973</v>
+        <v>228.2228732935722</v>
       </c>
       <c r="O11">
-        <v>6.484216255801467</v>
-      </c>
-    </row>
-    <row r="12" spans="1:30">
+        <v>7.643466364614945</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12">
-        <v>0.427135678</v>
+        <v>0.6884422109999999</v>
       </c>
       <c r="D12">
-        <v>0.540983607</v>
+        <v>0.327868852</v>
       </c>
       <c r="E12">
-        <v>0.292929293</v>
+        <v>0.353535354</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>0.19858156</v>
       </c>
       <c r="G12">
-        <v>0.396423249</v>
+        <v>0.642324888</v>
       </c>
       <c r="H12">
-        <v>0.116567037</v>
+        <v>0.943637916</v>
       </c>
       <c r="I12">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K12" t="s">
         <v>12</v>
       </c>
       <c r="L12">
-        <v>33.774038864</v>
+        <v>36.154390781</v>
       </c>
       <c r="M12">
-        <v>0.4454555536624887</v>
+        <v>0.4967770402230923</v>
       </c>
       <c r="N12">
-        <v>155.5228900833753</v>
+        <v>172.4093614298593</v>
       </c>
       <c r="O12">
-        <v>5.811543587034343</v>
-      </c>
-    </row>
-    <row r="13" spans="1:30">
+        <v>6.012852133638411</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C13">
-        <v>0.447236181</v>
+        <v>1.432160804</v>
       </c>
       <c r="D13">
-        <v>0.540983607</v>
+        <v>0.9180327859999999</v>
       </c>
       <c r="E13">
-        <v>0.232323232</v>
+        <v>0.707070708</v>
       </c>
       <c r="F13">
-        <v>0.111111111</v>
+        <v>0.19858156</v>
       </c>
       <c r="G13">
-        <v>0.418777943</v>
+        <v>1.143070044</v>
       </c>
       <c r="H13">
-        <v>0.038001708</v>
+        <v>1.178052946</v>
       </c>
       <c r="I13">
-        <v>21</v>
+        <v>83</v>
       </c>
       <c r="J13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K13" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="L13">
-        <v>23.788433782</v>
+        <v>94.57696884800001</v>
       </c>
       <c r="M13">
-        <v>0.3968520662051606</v>
+        <v>1.130450812772941</v>
       </c>
       <c r="N13">
-        <v>140.7546366721272</v>
+        <v>400.6322347234315</v>
       </c>
       <c r="O13">
-        <v>4.877338801231672</v>
-      </c>
-    </row>
-    <row r="14" spans="1:30">
+        <v>13.65631849825336</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14">
         <v>1</v>
       </c>
@@ -64226,289 +64190,289 @@
         <v>5.811543587034343</v>
       </c>
     </row>
-    <row r="15" spans="1:30">
+    <row r="15" spans="1:15">
       <c r="A15">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C15">
-        <v>0.6884422109999999</v>
+        <v>0.91959799</v>
       </c>
       <c r="D15">
-        <v>0.327868852</v>
+        <v>0.524590164</v>
       </c>
       <c r="E15">
-        <v>0.353535354</v>
+        <v>0</v>
       </c>
       <c r="F15">
-        <v>0.19858156</v>
+        <v>0</v>
       </c>
       <c r="G15">
-        <v>0.642324888</v>
+        <v>0.347242921</v>
       </c>
       <c r="H15">
-        <v>0.943637916</v>
+        <v>0.253629377</v>
       </c>
       <c r="I15">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J15">
         <v>1</v>
       </c>
       <c r="K15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L15">
-        <v>36.154390781</v>
+        <v>42.045060452</v>
       </c>
       <c r="M15">
-        <v>0.4967770402230923</v>
+        <v>0.6386575851883864</v>
       </c>
       <c r="N15">
-        <v>172.4093614298593</v>
+        <v>230.6932436063973</v>
       </c>
       <c r="O15">
-        <v>6.012852133638411</v>
-      </c>
-    </row>
-    <row r="16" spans="1:30">
+        <v>6.484216255801467</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B16">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C16">
-        <v>0.91959799</v>
+        <v>1.346733668</v>
       </c>
       <c r="D16">
-        <v>0.524590164</v>
+        <v>1.065573771</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>0.292929293</v>
       </c>
       <c r="F16">
         <v>0</v>
       </c>
       <c r="G16">
-        <v>0.347242921</v>
+        <v>0.74366617</v>
       </c>
       <c r="H16">
-        <v>0.253629377</v>
+        <v>0.370196414</v>
       </c>
       <c r="I16">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="J16">
         <v>1</v>
       </c>
       <c r="K16" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="L16">
-        <v>42.045060452</v>
+        <v>75.81909931600001</v>
       </c>
       <c r="M16">
-        <v>0.6386575851883864</v>
+        <v>1.084113138850875</v>
       </c>
       <c r="N16">
-        <v>230.6932436063973</v>
+        <v>386.2161336897726</v>
       </c>
       <c r="O16">
-        <v>6.484216255801467</v>
-      </c>
-    </row>
-    <row r="17" spans="1:30">
+        <v>12.29575984283581</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
       <c r="A17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17">
-        <v>0.447236181</v>
+        <v>0.427135678</v>
       </c>
       <c r="D17">
         <v>0.540983607</v>
       </c>
       <c r="E17">
+        <v>0.292929293</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0.396423249</v>
+      </c>
+      <c r="H17">
+        <v>0.116567037</v>
+      </c>
+      <c r="I17">
+        <v>31</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17" t="s">
+        <v>12</v>
+      </c>
+      <c r="L17">
+        <v>33.774038864</v>
+      </c>
+      <c r="M17">
+        <v>0.4454555536624887</v>
+      </c>
+      <c r="N17">
+        <v>155.5228900833753</v>
+      </c>
+      <c r="O17">
+        <v>5.811543587034343</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
+      <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>0.447236181</v>
+      </c>
+      <c r="D18">
+        <v>0.540983607</v>
+      </c>
+      <c r="E18">
         <v>0.232323232</v>
       </c>
-      <c r="F17">
+      <c r="F18">
         <v>0.111111111</v>
       </c>
-      <c r="G17">
+      <c r="G18">
         <v>0.418777943</v>
       </c>
-      <c r="H17">
+      <c r="H18">
         <v>0.038001708</v>
       </c>
-      <c r="I17">
+      <c r="I18">
         <v>21</v>
       </c>
-      <c r="J17">
-        <v>0</v>
-      </c>
-      <c r="K17" t="s">
-        <v>11</v>
-      </c>
-      <c r="L17">
-        <v>23.788433782</v>
-      </c>
-      <c r="M17">
-        <v>0.3968520662051606</v>
-      </c>
-      <c r="N17">
-        <v>140.7546366721272</v>
-      </c>
-      <c r="O17">
-        <v>4.877338801231672</v>
-      </c>
-    </row>
-    <row r="18" spans="1:30">
-      <c r="A18">
-        <v>2</v>
-      </c>
-      <c r="B18">
-        <v>8</v>
-      </c>
-      <c r="C18">
-        <v>0.91959799</v>
-      </c>
-      <c r="D18">
-        <v>0.524590164</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <v>0.347242921</v>
-      </c>
-      <c r="H18">
-        <v>0.253629377</v>
-      </c>
-      <c r="I18">
-        <v>32</v>
-      </c>
       <c r="J18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K18" t="s">
         <v>11</v>
       </c>
       <c r="L18">
-        <v>42.045060452</v>
+        <v>23.788433782</v>
       </c>
       <c r="M18">
-        <v>0.6386575851883864</v>
+        <v>0.3968520662051606</v>
       </c>
       <c r="N18">
-        <v>230.6932436063973</v>
+        <v>140.7546366721272</v>
       </c>
       <c r="O18">
-        <v>6.484216255801467</v>
-      </c>
-    </row>
-    <row r="19" spans="1:30">
+        <v>4.877338801231672</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
       <c r="A19">
         <v>4</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C19">
-        <v>0.6884422109999999</v>
+        <v>0.874371859</v>
       </c>
       <c r="D19">
-        <v>0.327868852</v>
+        <v>1.081967214</v>
       </c>
       <c r="E19">
-        <v>0.353535354</v>
+        <v>0.525252525</v>
       </c>
       <c r="F19">
-        <v>0.19858156</v>
+        <v>0.111111111</v>
       </c>
       <c r="G19">
-        <v>0.642324888</v>
+        <v>0.815201192</v>
       </c>
       <c r="H19">
-        <v>0.943637916</v>
+        <v>0.154568745</v>
       </c>
       <c r="I19">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="J19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K19" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="L19">
-        <v>36.154390781</v>
+        <v>57.562472646</v>
       </c>
       <c r="M19">
-        <v>0.4967770402230923</v>
+        <v>0.8423076198676492</v>
       </c>
       <c r="N19">
-        <v>172.4093614298593</v>
+        <v>296.2775267555025</v>
       </c>
       <c r="O19">
-        <v>6.012852133638411</v>
-      </c>
-    </row>
-    <row r="20" spans="1:30">
+        <v>10.68888238826602</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
       <c r="A20">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20">
-        <v>0.447236181</v>
+        <v>0.427135678</v>
       </c>
       <c r="D20">
         <v>0.540983607</v>
       </c>
       <c r="E20">
-        <v>0.232323232</v>
+        <v>0.292929293</v>
       </c>
       <c r="F20">
-        <v>0.111111111</v>
+        <v>0</v>
       </c>
       <c r="G20">
-        <v>0.418777943</v>
+        <v>0.396423249</v>
       </c>
       <c r="H20">
-        <v>0.038001708</v>
+        <v>0.116567037</v>
       </c>
       <c r="I20">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="J20">
         <v>0</v>
       </c>
       <c r="K20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L20">
-        <v>23.788433782</v>
+        <v>33.774038864</v>
       </c>
       <c r="M20">
-        <v>0.3968520662051606</v>
+        <v>0.4454555536624887</v>
       </c>
       <c r="N20">
-        <v>140.7546366721272</v>
+        <v>155.5228900833753</v>
       </c>
       <c r="O20">
-        <v>4.877338801231672</v>
-      </c>
-    </row>
-    <row r="21" spans="1:30">
+        <v>5.811543587034343</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
       <c r="A21">
         <v>4</v>
       </c>
@@ -64555,50 +64519,473 @@
         <v>6.012852133638411</v>
       </c>
     </row>
-    <row r="22" spans="1:30">
-      <c r="P22">
+    <row r="22" spans="1:15">
+      <c r="A22">
+        <v>5</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>1.115577889</v>
+      </c>
+      <c r="D22">
+        <v>0.868852459</v>
+      </c>
+      <c r="E22">
+        <v>0.6464646469999999</v>
+      </c>
+      <c r="F22">
+        <v>0.19858156</v>
+      </c>
+      <c r="G22">
+        <v>1.038748137</v>
+      </c>
+      <c r="H22">
+        <v>1.060204953</v>
+      </c>
+      <c r="I22">
+        <v>64</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+      <c r="K22" t="s">
+        <v>22</v>
+      </c>
+      <c r="L22">
+        <v>69.92842964499999</v>
+      </c>
+      <c r="M22">
+        <v>0.942232593885581</v>
+      </c>
+      <c r="N22">
+        <v>327.9322515132346</v>
+      </c>
+      <c r="O22">
+        <v>11.82439572067275</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23">
+        <v>8</v>
+      </c>
+      <c r="C23">
+        <v>0.91959799</v>
+      </c>
+      <c r="D23">
+        <v>0.524590164</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0.347242921</v>
+      </c>
+      <c r="H23">
+        <v>0.253629377</v>
+      </c>
+      <c r="I23">
+        <v>32</v>
+      </c>
+      <c r="J23">
+        <v>1</v>
+      </c>
+      <c r="K23" t="s">
+        <v>11</v>
+      </c>
+      <c r="L23">
+        <v>42.045060452</v>
+      </c>
+      <c r="M23">
+        <v>0.6386575851883864</v>
+      </c>
+      <c r="N23">
+        <v>230.6932436063973</v>
+      </c>
+      <c r="O23">
+        <v>6.484216255801467</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="A24">
+        <v>3</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>0.447236181</v>
+      </c>
+      <c r="D24">
+        <v>0.540983607</v>
+      </c>
+      <c r="E24">
+        <v>0.232323232</v>
+      </c>
+      <c r="F24">
+        <v>0.111111111</v>
+      </c>
+      <c r="G24">
+        <v>0.418777943</v>
+      </c>
+      <c r="H24">
+        <v>0.038001708</v>
+      </c>
+      <c r="I24">
+        <v>21</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24" t="s">
+        <v>11</v>
+      </c>
+      <c r="L24">
+        <v>23.788433782</v>
+      </c>
+      <c r="M24">
+        <v>0.3968520662051606</v>
+      </c>
+      <c r="N24">
+        <v>140.7546366721272</v>
+      </c>
+      <c r="O24">
+        <v>4.877338801231672</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="A25">
+        <v>5</v>
+      </c>
+      <c r="B25">
+        <v>9</v>
+      </c>
+      <c r="C25">
+        <v>1.366834171</v>
+      </c>
+      <c r="D25">
+        <v>1.065573771</v>
+      </c>
+      <c r="E25">
+        <v>0.232323232</v>
+      </c>
+      <c r="F25">
+        <v>0.111111111</v>
+      </c>
+      <c r="G25">
+        <v>0.7660208639999999</v>
+      </c>
+      <c r="H25">
+        <v>0.291631085</v>
+      </c>
+      <c r="I25">
+        <v>53</v>
+      </c>
+      <c r="J25">
+        <v>1</v>
+      </c>
+      <c r="K25" t="s">
+        <v>20</v>
+      </c>
+      <c r="L25">
+        <v>65.833494234</v>
+      </c>
+      <c r="M25">
+        <v>1.035509651393547</v>
+      </c>
+      <c r="N25">
+        <v>371.4478802785245</v>
+      </c>
+      <c r="O25">
+        <v>11.36155505703314</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="A26">
+        <v>2</v>
+      </c>
+      <c r="B26">
+        <v>8</v>
+      </c>
+      <c r="C26">
+        <v>0.91959799</v>
+      </c>
+      <c r="D26">
+        <v>0.524590164</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0.347242921</v>
+      </c>
+      <c r="H26">
+        <v>0.253629377</v>
+      </c>
+      <c r="I26">
+        <v>32</v>
+      </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
+      <c r="K26" t="s">
+        <v>11</v>
+      </c>
+      <c r="L26">
+        <v>42.045060452</v>
+      </c>
+      <c r="M26">
+        <v>0.6386575851883864</v>
+      </c>
+      <c r="N26">
+        <v>230.6932436063973</v>
+      </c>
+      <c r="O26">
+        <v>6.484216255801467</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
+      <c r="A27">
+        <v>4</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0.6884422109999999</v>
+      </c>
+      <c r="D27">
+        <v>0.327868852</v>
+      </c>
+      <c r="E27">
+        <v>0.353535354</v>
+      </c>
+      <c r="F27">
+        <v>0.19858156</v>
+      </c>
+      <c r="G27">
+        <v>0.642324888</v>
+      </c>
+      <c r="H27">
+        <v>0.943637916</v>
+      </c>
+      <c r="I27">
+        <v>33</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="K27" t="s">
+        <v>12</v>
+      </c>
+      <c r="L27">
+        <v>36.154390781</v>
+      </c>
+      <c r="M27">
+        <v>0.4967770402230923</v>
+      </c>
+      <c r="N27">
+        <v>172.4093614298593</v>
+      </c>
+      <c r="O27">
+        <v>6.012852133638411</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="A28">
+        <v>6</v>
+      </c>
+      <c r="B28">
+        <v>8</v>
+      </c>
+      <c r="C28">
+        <v>1.608040201</v>
+      </c>
+      <c r="D28">
+        <v>0.8524590160000001</v>
+      </c>
+      <c r="E28">
+        <v>0.353535354</v>
+      </c>
+      <c r="F28">
+        <v>0.19858156</v>
+      </c>
+      <c r="G28">
+        <v>0.989567809</v>
+      </c>
+      <c r="H28">
+        <v>1.197267293</v>
+      </c>
+      <c r="I28">
+        <v>65</v>
+      </c>
+      <c r="J28">
+        <v>2</v>
+      </c>
+      <c r="K28" t="s">
+        <v>19</v>
+      </c>
+      <c r="L28">
+        <v>78.19945123299999</v>
+      </c>
+      <c r="M28">
+        <v>1.135434625411479</v>
+      </c>
+      <c r="N28">
+        <v>403.1026050362566</v>
+      </c>
+      <c r="O28">
+        <v>12.49706838943988</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15">
+      <c r="A29">
+        <v>3</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>0.447236181</v>
+      </c>
+      <c r="D29">
+        <v>0.540983607</v>
+      </c>
+      <c r="E29">
+        <v>0.232323232</v>
+      </c>
+      <c r="F29">
+        <v>0.111111111</v>
+      </c>
+      <c r="G29">
+        <v>0.418777943</v>
+      </c>
+      <c r="H29">
+        <v>0.038001708</v>
+      </c>
+      <c r="I29">
+        <v>21</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29" t="s">
+        <v>11</v>
+      </c>
+      <c r="L29">
+        <v>23.788433782</v>
+      </c>
+      <c r="M29">
+        <v>0.3968520662051606</v>
+      </c>
+      <c r="N29">
+        <v>140.7546366721272</v>
+      </c>
+      <c r="O29">
+        <v>4.877338801231672</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15">
+      <c r="A30">
+        <v>4</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>0.6884422109999999</v>
+      </c>
+      <c r="D30">
+        <v>0.327868852</v>
+      </c>
+      <c r="E30">
+        <v>0.353535354</v>
+      </c>
+      <c r="F30">
+        <v>0.19858156</v>
+      </c>
+      <c r="G30">
+        <v>0.642324888</v>
+      </c>
+      <c r="H30">
+        <v>0.943637916</v>
+      </c>
+      <c r="I30">
+        <v>33</v>
+      </c>
+      <c r="J30">
+        <v>1</v>
+      </c>
+      <c r="K30" t="s">
+        <v>12</v>
+      </c>
+      <c r="L30">
+        <v>36.154390781</v>
+      </c>
+      <c r="M30">
+        <v>0.4967770402230923</v>
+      </c>
+      <c r="N30">
+        <v>172.4093614298593</v>
+      </c>
+      <c r="O30">
+        <v>6.012852133638411</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15">
+      <c r="A31">
         <v>7</v>
       </c>
-      <c r="Q22">
-        <v>1</v>
-      </c>
-      <c r="R22">
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
         <v>1.135678392</v>
       </c>
-      <c r="S22">
+      <c r="D31">
         <v>0.868852459</v>
       </c>
-      <c r="T22">
+      <c r="E31">
         <v>0.5858585860000001</v>
       </c>
-      <c r="U22">
+      <c r="F31">
         <v>0.309692671</v>
       </c>
-      <c r="V22">
+      <c r="G31">
         <v>1.061102831</v>
       </c>
-      <c r="W22">
+      <c r="H31">
         <v>0.981639624</v>
       </c>
-      <c r="X22">
+      <c r="I31">
         <v>54</v>
       </c>
-      <c r="Y22">
-        <v>1</v>
-      </c>
-      <c r="Z22" t="s">
+      <c r="J31">
+        <v>1</v>
+      </c>
+      <c r="K31" t="s">
         <v>19</v>
       </c>
-      <c r="AA22">
+      <c r="L31">
         <v>59.942824563</v>
       </c>
-      <c r="AB22">
+      <c r="M31">
         <v>0.8936291064282529</v>
       </c>
-      <c r="AC22">
+      <c r="N31">
         <v>313.1639981019865</v>
       </c>
-      <c r="AD22">
+      <c r="O31">
         <v>10.89019093487008</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Computed value of error and closeness factor
</commit_message>
<xml_diff>
--- a/diabetes_data.xlsx
+++ b/diabetes_data.xlsx
@@ -10,13 +10,18 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Error" sheetId="4" r:id="rId4"/>
+    <sheet name="Error sq" sheetId="5" r:id="rId5"/>
+    <sheet name="Weight" sheetId="6" r:id="rId6"/>
+    <sheet name="Error sq x Weight" sheetId="7" r:id="rId7"/>
+    <sheet name="Closeness Factor" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1607" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1637" uniqueCount="24">
   <si>
     <t>Index</t>
   </si>
@@ -85,6 +90,9 @@
   </si>
   <si>
     <t>CC</t>
+  </si>
+  <si>
+    <t>-inf</t>
   </si>
 </sst>
 </file>
@@ -64992,4 +65000,228 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>